<commit_message>
account project and user
</commit_message>
<xml_diff>
--- a/public/uploads/xlsforms/Student ODK formV3.xlsx
+++ b/public/uploads/xlsforms/Student ODK formV3.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LuciaFalcinelli\Documents\GitHub\ccrp_soils_laravel\public\uploads\xlsforms\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LuciaFalcinelli\Dropbox (SSD)\Unicef\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AD6281B-A936-4581-8E88-FE9F2933D8D7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FA7ABF8-9A46-4D97-BE98-61D03329546A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11385" xr2:uid="{7F77898F-92E8-4B75-B8B4-C3EC08824587}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392" xr2:uid="{7F77898F-92E8-4B75-B8B4-C3EC08824587}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
     <sheet name="choices" sheetId="2" r:id="rId2"/>
     <sheet name="settings" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1571" uniqueCount="806">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1564" uniqueCount="802">
   <si>
     <t>type</t>
   </si>
@@ -2445,18 +2445,6 @@
   </si>
   <si>
     <t>selected(${change_pads_school}, '1') and selected(${period_started}, '1')</t>
-  </si>
-  <si>
-    <t>testing</t>
-  </si>
-  <si>
-    <t>Replace</t>
-  </si>
-  <si>
-    <t>villageTEST</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> VILLAGTESTE</t>
   </si>
 </sst>
 </file>
@@ -2914,12 +2902,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7E63475-E550-48C8-BF8A-60811DA3E4BE}">
-  <dimension ref="A1:I179"/>
+  <dimension ref="A1:I177"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A88" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
+      <selection pane="bottomLeft" activeCell="H90" sqref="H90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3012,29 +3000,32 @@
       <c r="E5" s="9"/>
       <c r="F5" s="10"/>
     </row>
-    <row r="6" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>802</v>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>803</v>
+        <v>16</v>
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="9"/>
       <c r="F6" s="10"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I6" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>804</v>
+        <v>18</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>805</v>
+        <v>19</v>
       </c>
       <c r="D7" s="8"/>
       <c r="E7" s="9"/>
@@ -3045,13 +3036,13 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="D8" s="8"/>
       <c r="E8" s="9"/>
@@ -3060,15 +3051,15 @@
         <v>797</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>89</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>401</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>19</v>
+        <v>90</v>
       </c>
       <c r="D9" s="8"/>
       <c r="E9" s="9"/>
@@ -3079,13 +3070,13 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>91</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>92</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>22</v>
+        <v>93</v>
       </c>
       <c r="D10" s="8"/>
       <c r="E10" s="9"/>
@@ -3096,13 +3087,13 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="B11" t="s">
-        <v>401</v>
+        <v>62</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>90</v>
+        <v>102</v>
       </c>
       <c r="D11" s="8"/>
       <c r="E11" s="9"/>
@@ -3111,15 +3102,12 @@
         <v>797</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="195" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>91</v>
-      </c>
-      <c r="B12" t="s">
-        <v>92</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>93</v>
+        <v>103</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>576</v>
       </c>
       <c r="D12" s="8"/>
       <c r="E12" s="9"/>
@@ -3130,13 +3118,10 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>101</v>
-      </c>
-      <c r="B13" t="s">
-        <v>62</v>
+        <v>103</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="D13" s="8"/>
       <c r="E13" s="9"/>
@@ -3145,12 +3130,15 @@
         <v>797</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="195" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>103</v>
-      </c>
-      <c r="C14" s="15" t="s">
-        <v>576</v>
+        <v>105</v>
+      </c>
+      <c r="B14" t="s">
+        <v>86</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>106</v>
       </c>
       <c r="D14" s="8"/>
       <c r="E14" s="9"/>
@@ -3159,13 +3147,11 @@
         <v>797</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>103</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>104</v>
-      </c>
+    <row r="15" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="C15" s="7"/>
       <c r="D15" s="8"/>
       <c r="E15" s="9"/>
       <c r="F15" s="10"/>
@@ -3173,28 +3159,36 @@
         <v>797</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>105</v>
-      </c>
-      <c r="B16" t="s">
-        <v>86</v>
+    <row r="16" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>108</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="D16" s="8"/>
       <c r="E16" s="9"/>
       <c r="F16" s="10"/>
+      <c r="H16" s="11" t="s">
+        <v>110</v>
+      </c>
       <c r="I16" t="s">
         <v>797</v>
       </c>
     </row>
-    <row r="17" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="16" t="s">
-        <v>107</v>
-      </c>
-      <c r="C17" s="7"/>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>116</v>
+      </c>
+      <c r="B17" t="s">
+        <v>113</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>112</v>
+      </c>
       <c r="D17" s="8"/>
       <c r="E17" s="9"/>
       <c r="F17" s="10"/>
@@ -3202,35 +3196,32 @@
         <v>797</v>
       </c>
     </row>
-    <row r="18" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B18" s="11" t="s">
-        <v>108</v>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>100</v>
+      </c>
+      <c r="B18" t="s">
+        <v>118</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="D18" s="8"/>
       <c r="E18" s="9"/>
       <c r="F18" s="10"/>
-      <c r="H18" s="11" t="s">
-        <v>110</v>
-      </c>
       <c r="I18" t="s">
         <v>797</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="B19" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="D19" s="8"/>
       <c r="E19" s="9"/>
@@ -3239,16 +3230,11 @@
         <v>797</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>100</v>
-      </c>
-      <c r="B20" t="s">
-        <v>118</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>117</v>
-      </c>
+    <row r="20" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="C20" s="7"/>
       <c r="D20" s="8"/>
       <c r="E20" s="9"/>
       <c r="F20" s="10"/>
@@ -3256,50 +3242,49 @@
         <v>797</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>100</v>
-      </c>
-      <c r="B21" t="s">
-        <v>119</v>
+    <row r="21" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>406</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>120</v>
+        <v>405</v>
       </c>
       <c r="D21" s="8"/>
       <c r="E21" s="9"/>
       <c r="F21" s="10"/>
+      <c r="H21" s="11" t="s">
+        <v>110</v>
+      </c>
       <c r="I21" t="s">
         <v>797</v>
       </c>
     </row>
-    <row r="22" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="16" t="s">
-        <v>107</v>
-      </c>
-      <c r="C22" s="7"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="10"/>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>135</v>
+      </c>
+      <c r="B22" t="s">
+        <v>141</v>
+      </c>
+      <c r="C22" t="s">
+        <v>140</v>
+      </c>
       <c r="I22" t="s">
         <v>797</v>
       </c>
     </row>
-    <row r="23" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B23" s="11" t="s">
-        <v>406</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>405</v>
-      </c>
-      <c r="D23" s="8"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="10"/>
-      <c r="H23" s="11" t="s">
-        <v>110</v>
+    <row r="23" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>134</v>
+      </c>
+      <c r="B23" t="s">
+        <v>143</v>
+      </c>
+      <c r="C23" s="17" t="s">
+        <v>142</v>
       </c>
       <c r="I23" t="s">
         <v>797</v>
@@ -3307,27 +3292,36 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
       <c r="B24" t="s">
-        <v>141</v>
-      </c>
-      <c r="C24" t="s">
-        <v>140</v>
+        <v>145</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="H24" t="s">
+        <v>155</v>
       </c>
       <c r="I24" t="s">
         <v>797</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>134</v>
+        <v>89</v>
       </c>
       <c r="B25" t="s">
-        <v>143</v>
-      </c>
-      <c r="C25" s="17" t="s">
-        <v>142</v>
+        <v>154</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="D25" s="8"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="10"/>
+      <c r="H25" t="s">
+        <v>152</v>
       </c>
       <c r="I25" t="s">
         <v>797</v>
@@ -3335,16 +3329,19 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="B26" t="s">
-        <v>145</v>
+        <v>409</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>144</v>
-      </c>
+        <v>407</v>
+      </c>
+      <c r="D26" s="8"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="10"/>
       <c r="H26" t="s">
-        <v>155</v>
+        <v>408</v>
       </c>
       <c r="I26" t="s">
         <v>797</v>
@@ -3352,19 +3349,19 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>89</v>
+        <v>134</v>
       </c>
       <c r="B27" t="s">
-        <v>154</v>
+        <v>413</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>111</v>
+        <v>410</v>
       </c>
       <c r="D27" s="8"/>
       <c r="E27" s="9"/>
       <c r="F27" s="10"/>
       <c r="H27" t="s">
-        <v>152</v>
+        <v>408</v>
       </c>
       <c r="I27" t="s">
         <v>797</v>
@@ -3375,10 +3372,10 @@
         <v>134</v>
       </c>
       <c r="B28" t="s">
-        <v>409</v>
+        <v>414</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>407</v>
+        <v>411</v>
       </c>
       <c r="D28" s="8"/>
       <c r="E28" s="9"/>
@@ -3395,10 +3392,10 @@
         <v>134</v>
       </c>
       <c r="B29" t="s">
-        <v>413</v>
+        <v>415</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="D29" s="8"/>
       <c r="E29" s="9"/>
@@ -3410,99 +3407,96 @@
         <v>797</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>134</v>
-      </c>
-      <c r="B30" t="s">
-        <v>414</v>
-      </c>
-      <c r="C30" s="7" t="s">
-        <v>411</v>
-      </c>
+    <row r="30" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="C30" s="7"/>
       <c r="D30" s="8"/>
       <c r="E30" s="9"/>
       <c r="F30" s="10"/>
-      <c r="H30" t="s">
-        <v>408</v>
-      </c>
       <c r="I30" t="s">
         <v>797</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>134</v>
-      </c>
-      <c r="B31" t="s">
-        <v>415</v>
+    <row r="31" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B31" s="11" t="s">
+        <v>161</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>412</v>
+        <v>162</v>
       </c>
       <c r="D31" s="8"/>
       <c r="E31" s="9"/>
       <c r="F31" s="10"/>
-      <c r="H31" t="s">
-        <v>408</v>
+      <c r="H31" s="11" t="s">
+        <v>110</v>
       </c>
       <c r="I31" t="s">
         <v>797</v>
       </c>
     </row>
-    <row r="32" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="16" t="s">
-        <v>107</v>
-      </c>
-      <c r="C32" s="7"/>
-      <c r="D32" s="8"/>
-      <c r="E32" s="9"/>
-      <c r="F32" s="10"/>
+    <row r="32" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="C32" s="17" t="s">
+        <v>163</v>
+      </c>
+      <c r="D32" s="17"/>
       <c r="I32" t="s">
         <v>797</v>
       </c>
     </row>
-    <row r="33" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B33" s="11" t="s">
-        <v>161</v>
-      </c>
-      <c r="C33" s="7" t="s">
-        <v>162</v>
-      </c>
-      <c r="D33" s="8"/>
-      <c r="E33" s="9"/>
-      <c r="F33" s="10"/>
-      <c r="H33" s="11" t="s">
-        <v>110</v>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>134</v>
+      </c>
+      <c r="B33" t="s">
+        <v>164</v>
+      </c>
+      <c r="C33" t="s">
+        <v>418</v>
       </c>
       <c r="I33" t="s">
         <v>797</v>
       </c>
     </row>
-    <row r="34" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="18" t="s">
-        <v>103</v>
-      </c>
-      <c r="C34" s="17" t="s">
-        <v>163</v>
-      </c>
-      <c r="D34" s="17"/>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>165</v>
+      </c>
+      <c r="B34" t="s">
+        <v>166</v>
+      </c>
+      <c r="C34" t="s">
+        <v>419</v>
+      </c>
+      <c r="H34" t="s">
+        <v>416</v>
+      </c>
       <c r="I34" t="s">
         <v>797</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>134</v>
+        <v>89</v>
       </c>
       <c r="B35" t="s">
-        <v>164</v>
-      </c>
-      <c r="C35" t="s">
-        <v>418</v>
+        <v>172</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="D35" s="8"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="10"/>
+      <c r="H35" t="s">
+        <v>173</v>
       </c>
       <c r="I35" t="s">
         <v>797</v>
@@ -3510,16 +3504,16 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>165</v>
+        <v>175</v>
       </c>
       <c r="B36" t="s">
-        <v>166</v>
+        <v>174</v>
       </c>
       <c r="C36" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="H36" t="s">
-        <v>416</v>
+        <v>798</v>
       </c>
       <c r="I36" t="s">
         <v>797</v>
@@ -3530,7 +3524,7 @@
         <v>89</v>
       </c>
       <c r="B37" t="s">
-        <v>172</v>
+        <v>180</v>
       </c>
       <c r="C37" s="7" t="s">
         <v>111</v>
@@ -3539,7 +3533,7 @@
       <c r="E37" s="9"/>
       <c r="F37" s="10"/>
       <c r="H37" t="s">
-        <v>173</v>
+        <v>181</v>
       </c>
       <c r="I37" t="s">
         <v>797</v>
@@ -3547,17 +3541,17 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>175</v>
+        <v>422</v>
       </c>
       <c r="B38" t="s">
-        <v>174</v>
-      </c>
-      <c r="C38" t="s">
-        <v>420</v>
-      </c>
-      <c r="H38" t="s">
-        <v>798</v>
-      </c>
+        <v>423</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>421</v>
+      </c>
+      <c r="D38" s="8"/>
+      <c r="E38" s="9"/>
+      <c r="F38" s="10"/>
       <c r="I38" t="s">
         <v>797</v>
       </c>
@@ -3567,7 +3561,7 @@
         <v>89</v>
       </c>
       <c r="B39" t="s">
-        <v>180</v>
+        <v>429</v>
       </c>
       <c r="C39" s="7" t="s">
         <v>111</v>
@@ -3576,7 +3570,7 @@
       <c r="E39" s="9"/>
       <c r="F39" s="10"/>
       <c r="H39" t="s">
-        <v>181</v>
+        <v>430</v>
       </c>
       <c r="I39" t="s">
         <v>797</v>
@@ -3584,36 +3578,30 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>422</v>
+        <v>134</v>
       </c>
       <c r="B40" t="s">
-        <v>423</v>
-      </c>
-      <c r="C40" s="7" t="s">
-        <v>421</v>
-      </c>
-      <c r="D40" s="8"/>
-      <c r="E40" s="9"/>
-      <c r="F40" s="10"/>
+        <v>183</v>
+      </c>
+      <c r="C40" t="s">
+        <v>182</v>
+      </c>
       <c r="I40" t="s">
         <v>797</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>89</v>
+        <v>186</v>
       </c>
       <c r="B41" t="s">
-        <v>429</v>
-      </c>
-      <c r="C41" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="D41" s="8"/>
-      <c r="E41" s="9"/>
-      <c r="F41" s="10"/>
+        <v>187</v>
+      </c>
+      <c r="C41" t="s">
+        <v>184</v>
+      </c>
       <c r="H41" t="s">
-        <v>430</v>
+        <v>185</v>
       </c>
       <c r="I41" t="s">
         <v>797</v>
@@ -3621,13 +3609,13 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>134</v>
+        <v>438</v>
       </c>
       <c r="B42" t="s">
-        <v>183</v>
-      </c>
-      <c r="C42" t="s">
-        <v>182</v>
+        <v>437</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>436</v>
       </c>
       <c r="I42" t="s">
         <v>797</v>
@@ -3635,16 +3623,19 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>186</v>
+        <v>89</v>
       </c>
       <c r="B43" t="s">
-        <v>187</v>
-      </c>
-      <c r="C43" t="s">
-        <v>184</v>
-      </c>
+        <v>439</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="D43" s="8"/>
+      <c r="E43" s="9"/>
+      <c r="F43" s="10"/>
       <c r="H43" t="s">
-        <v>185</v>
+        <v>440</v>
       </c>
       <c r="I43" t="s">
         <v>797</v>
@@ -3652,13 +3643,16 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>438</v>
+        <v>217</v>
       </c>
       <c r="B44" t="s">
-        <v>437</v>
+        <v>442</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>436</v>
+        <v>441</v>
+      </c>
+      <c r="H44" t="s">
+        <v>443</v>
       </c>
       <c r="I44" t="s">
         <v>797</v>
@@ -3669,7 +3663,7 @@
         <v>89</v>
       </c>
       <c r="B45" t="s">
-        <v>439</v>
+        <v>444</v>
       </c>
       <c r="C45" s="7" t="s">
         <v>111</v>
@@ -3678,7 +3672,7 @@
       <c r="E45" s="9"/>
       <c r="F45" s="10"/>
       <c r="H45" t="s">
-        <v>440</v>
+        <v>445</v>
       </c>
       <c r="I45" t="s">
         <v>797</v>
@@ -3686,16 +3680,13 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>217</v>
+        <v>447</v>
       </c>
       <c r="B46" t="s">
-        <v>442</v>
-      </c>
-      <c r="C46" s="7" t="s">
-        <v>441</v>
-      </c>
-      <c r="H46" t="s">
-        <v>443</v>
+        <v>448</v>
+      </c>
+      <c r="C46" t="s">
+        <v>446</v>
       </c>
       <c r="I46" t="s">
         <v>797</v>
@@ -3703,19 +3694,16 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>89</v>
+        <v>465</v>
       </c>
       <c r="B47" t="s">
-        <v>444</v>
-      </c>
-      <c r="C47" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="D47" s="8"/>
-      <c r="E47" s="9"/>
-      <c r="F47" s="10"/>
+        <v>463</v>
+      </c>
+      <c r="C47" t="s">
+        <v>451</v>
+      </c>
       <c r="H47" t="s">
-        <v>445</v>
+        <v>462</v>
       </c>
       <c r="I47" t="s">
         <v>797</v>
@@ -3723,13 +3711,19 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>447</v>
+        <v>89</v>
       </c>
       <c r="B48" t="s">
-        <v>448</v>
-      </c>
-      <c r="C48" t="s">
-        <v>446</v>
+        <v>464</v>
+      </c>
+      <c r="C48" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="D48" s="8"/>
+      <c r="E48" s="9"/>
+      <c r="F48" s="10"/>
+      <c r="H48" t="s">
+        <v>466</v>
       </c>
       <c r="I48" t="s">
         <v>797</v>
@@ -3737,36 +3731,36 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>465</v>
+        <v>447</v>
       </c>
       <c r="B49" t="s">
-        <v>463</v>
-      </c>
-      <c r="C49" t="s">
-        <v>451</v>
-      </c>
-      <c r="H49" t="s">
-        <v>462</v>
-      </c>
+        <v>790</v>
+      </c>
+      <c r="C49" s="7" t="s">
+        <v>467</v>
+      </c>
+      <c r="D49" s="8"/>
+      <c r="E49" s="9"/>
+      <c r="F49" s="10"/>
       <c r="I49" t="s">
         <v>797</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>89</v>
+        <v>465</v>
       </c>
       <c r="B50" t="s">
-        <v>464</v>
+        <v>791</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>111</v>
+        <v>468</v>
       </c>
       <c r="D50" s="8"/>
       <c r="E50" s="9"/>
       <c r="F50" s="10"/>
       <c r="H50" t="s">
-        <v>466</v>
+        <v>793</v>
       </c>
       <c r="I50" t="s">
         <v>797</v>
@@ -3774,37 +3768,37 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>447</v>
+        <v>89</v>
       </c>
       <c r="B51" t="s">
-        <v>790</v>
+        <v>792</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>467</v>
+        <v>111</v>
       </c>
       <c r="D51" s="8"/>
       <c r="E51" s="9"/>
       <c r="F51" s="10"/>
+      <c r="H51" t="s">
+        <v>789</v>
+      </c>
       <c r="I51" t="s">
         <v>797</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>465</v>
+        <v>470</v>
       </c>
       <c r="B52" t="s">
-        <v>791</v>
+        <v>472</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="D52" s="8"/>
       <c r="E52" s="9"/>
       <c r="F52" s="10"/>
-      <c r="H52" t="s">
-        <v>793</v>
-      </c>
       <c r="I52" t="s">
         <v>797</v>
       </c>
@@ -3814,7 +3808,7 @@
         <v>89</v>
       </c>
       <c r="B53" t="s">
-        <v>792</v>
+        <v>479</v>
       </c>
       <c r="C53" s="7" t="s">
         <v>111</v>
@@ -3823,7 +3817,7 @@
       <c r="E53" s="9"/>
       <c r="F53" s="10"/>
       <c r="H53" t="s">
-        <v>789</v>
+        <v>480</v>
       </c>
       <c r="I53" t="s">
         <v>797</v>
@@ -3831,17 +3825,14 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>470</v>
+        <v>190</v>
       </c>
       <c r="B54" t="s">
-        <v>472</v>
-      </c>
-      <c r="C54" s="7" t="s">
-        <v>469</v>
-      </c>
-      <c r="D54" s="8"/>
-      <c r="E54" s="9"/>
-      <c r="F54" s="10"/>
+        <v>189</v>
+      </c>
+      <c r="C54" t="s">
+        <v>481</v>
+      </c>
       <c r="I54" t="s">
         <v>797</v>
       </c>
@@ -3851,7 +3842,7 @@
         <v>89</v>
       </c>
       <c r="B55" t="s">
-        <v>479</v>
+        <v>198</v>
       </c>
       <c r="C55" s="7" t="s">
         <v>111</v>
@@ -3860,7 +3851,7 @@
       <c r="E55" s="9"/>
       <c r="F55" s="10"/>
       <c r="H55" t="s">
-        <v>480</v>
+        <v>197</v>
       </c>
       <c r="I55" t="s">
         <v>797</v>
@@ -3868,47 +3859,44 @@
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>190</v>
+        <v>134</v>
       </c>
       <c r="B56" t="s">
-        <v>189</v>
+        <v>199</v>
       </c>
       <c r="C56" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="I56" t="s">
         <v>797</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>89</v>
+        <v>487</v>
       </c>
       <c r="B57" t="s">
-        <v>198</v>
+        <v>488</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="D57" s="8"/>
-      <c r="E57" s="9"/>
-      <c r="F57" s="10"/>
-      <c r="H57" t="s">
-        <v>197</v>
+        <v>483</v>
       </c>
       <c r="I57" t="s">
         <v>797</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>134</v>
+        <v>487</v>
       </c>
       <c r="B58" t="s">
-        <v>199</v>
-      </c>
-      <c r="C58" t="s">
-        <v>482</v>
+        <v>492</v>
+      </c>
+      <c r="C58" s="7" t="s">
+        <v>489</v>
+      </c>
+      <c r="H58" t="s">
+        <v>408</v>
       </c>
       <c r="I58" t="s">
         <v>797</v>
@@ -3919,24 +3907,27 @@
         <v>487</v>
       </c>
       <c r="B59" t="s">
-        <v>488</v>
+        <v>493</v>
       </c>
       <c r="C59" s="7" t="s">
-        <v>483</v>
+        <v>490</v>
+      </c>
+      <c r="H59" t="s">
+        <v>408</v>
       </c>
       <c r="I59" t="s">
         <v>797</v>
       </c>
     </row>
-    <row r="60" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>487</v>
+        <v>134</v>
       </c>
       <c r="B60" t="s">
-        <v>492</v>
-      </c>
-      <c r="C60" s="7" t="s">
-        <v>489</v>
+        <v>200</v>
+      </c>
+      <c r="C60" t="s">
+        <v>491</v>
       </c>
       <c r="H60" t="s">
         <v>408</v>
@@ -3945,18 +3936,18 @@
         <v>797</v>
       </c>
     </row>
-    <row r="61" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>487</v>
+        <v>201</v>
       </c>
       <c r="B61" t="s">
-        <v>493</v>
-      </c>
-      <c r="C61" s="7" t="s">
-        <v>490</v>
+        <v>202</v>
+      </c>
+      <c r="C61" t="s">
+        <v>494</v>
       </c>
       <c r="H61" t="s">
-        <v>408</v>
+        <v>206</v>
       </c>
       <c r="I61" t="s">
         <v>797</v>
@@ -3964,53 +3955,50 @@
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>134</v>
+        <v>89</v>
       </c>
       <c r="B62" t="s">
-        <v>200</v>
-      </c>
-      <c r="C62" t="s">
-        <v>491</v>
-      </c>
+        <v>207</v>
+      </c>
+      <c r="C62" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="D62" s="8"/>
+      <c r="E62" s="9"/>
+      <c r="F62" s="10"/>
       <c r="H62" t="s">
+        <v>208</v>
+      </c>
+      <c r="I62" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>103</v>
+      </c>
+      <c r="C63" s="7" t="s">
+        <v>495</v>
+      </c>
+      <c r="H63" t="s">
         <v>408</v>
       </c>
-      <c r="I62" t="s">
-        <v>797</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>201</v>
-      </c>
-      <c r="B63" t="s">
-        <v>202</v>
-      </c>
-      <c r="C63" t="s">
-        <v>494</v>
-      </c>
-      <c r="H63" t="s">
-        <v>206</v>
-      </c>
       <c r="I63" t="s">
         <v>797</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>89</v>
+        <v>502</v>
       </c>
       <c r="B64" t="s">
-        <v>207</v>
+        <v>503</v>
       </c>
       <c r="C64" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="D64" s="8"/>
-      <c r="E64" s="9"/>
-      <c r="F64" s="10"/>
+        <v>496</v>
+      </c>
       <c r="H64" t="s">
-        <v>208</v>
+        <v>408</v>
       </c>
       <c r="I64" t="s">
         <v>797</v>
@@ -4018,10 +4006,13 @@
     </row>
     <row r="65" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>103</v>
+        <v>502</v>
+      </c>
+      <c r="B65" t="s">
+        <v>505</v>
       </c>
       <c r="C65" s="7" t="s">
-        <v>495</v>
+        <v>504</v>
       </c>
       <c r="H65" t="s">
         <v>408</v>
@@ -4035,10 +4026,10 @@
         <v>502</v>
       </c>
       <c r="B66" t="s">
-        <v>503</v>
+        <v>507</v>
       </c>
       <c r="C66" s="7" t="s">
-        <v>496</v>
+        <v>506</v>
       </c>
       <c r="H66" t="s">
         <v>408</v>
@@ -4052,10 +4043,10 @@
         <v>502</v>
       </c>
       <c r="B67" t="s">
-        <v>505</v>
+        <v>509</v>
       </c>
       <c r="C67" s="7" t="s">
-        <v>504</v>
+        <v>508</v>
       </c>
       <c r="H67" t="s">
         <v>408</v>
@@ -4069,10 +4060,10 @@
         <v>502</v>
       </c>
       <c r="B68" t="s">
-        <v>507</v>
+        <v>521</v>
       </c>
       <c r="C68" s="7" t="s">
-        <v>506</v>
+        <v>510</v>
       </c>
       <c r="H68" t="s">
         <v>408</v>
@@ -4086,10 +4077,10 @@
         <v>502</v>
       </c>
       <c r="B69" t="s">
-        <v>509</v>
+        <v>794</v>
       </c>
       <c r="C69" s="7" t="s">
-        <v>508</v>
+        <v>511</v>
       </c>
       <c r="H69" t="s">
         <v>408</v>
@@ -4098,15 +4089,15 @@
         <v>797</v>
       </c>
     </row>
-    <row r="70" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>502</v>
       </c>
       <c r="B70" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="C70" s="7" t="s">
-        <v>510</v>
+        <v>512</v>
       </c>
       <c r="H70" t="s">
         <v>408</v>
@@ -4115,15 +4106,15 @@
         <v>797</v>
       </c>
     </row>
-    <row r="71" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>502</v>
       </c>
       <c r="B71" t="s">
-        <v>794</v>
+        <v>523</v>
       </c>
       <c r="C71" s="7" t="s">
-        <v>511</v>
+        <v>513</v>
       </c>
       <c r="H71" t="s">
         <v>408</v>
@@ -4137,10 +4128,10 @@
         <v>502</v>
       </c>
       <c r="B72" t="s">
-        <v>522</v>
+        <v>524</v>
       </c>
       <c r="C72" s="7" t="s">
-        <v>512</v>
+        <v>514</v>
       </c>
       <c r="H72" t="s">
         <v>408</v>
@@ -4154,10 +4145,10 @@
         <v>502</v>
       </c>
       <c r="B73" t="s">
-        <v>523</v>
+        <v>526</v>
       </c>
       <c r="C73" s="7" t="s">
-        <v>513</v>
+        <v>515</v>
       </c>
       <c r="H73" t="s">
         <v>408</v>
@@ -4171,10 +4162,10 @@
         <v>502</v>
       </c>
       <c r="B74" t="s">
-        <v>524</v>
+        <v>795</v>
       </c>
       <c r="C74" s="7" t="s">
-        <v>514</v>
+        <v>516</v>
       </c>
       <c r="H74" t="s">
         <v>408</v>
@@ -4188,10 +4179,10 @@
         <v>502</v>
       </c>
       <c r="B75" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="C75" s="7" t="s">
-        <v>515</v>
+        <v>517</v>
       </c>
       <c r="H75" t="s">
         <v>408</v>
@@ -4205,10 +4196,10 @@
         <v>502</v>
       </c>
       <c r="B76" t="s">
-        <v>795</v>
+        <v>527</v>
       </c>
       <c r="C76" s="7" t="s">
-        <v>516</v>
+        <v>518</v>
       </c>
       <c r="H76" t="s">
         <v>408</v>
@@ -4219,16 +4210,16 @@
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>502</v>
+        <v>134</v>
       </c>
       <c r="B77" t="s">
-        <v>525</v>
+        <v>528</v>
       </c>
       <c r="C77" s="7" t="s">
-        <v>517</v>
+        <v>519</v>
       </c>
       <c r="H77" t="s">
-        <v>408</v>
+        <v>520</v>
       </c>
       <c r="I77" t="s">
         <v>797</v>
@@ -4236,16 +4227,16 @@
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>502</v>
+        <v>530</v>
       </c>
       <c r="B78" t="s">
-        <v>527</v>
+        <v>531</v>
       </c>
       <c r="C78" s="7" t="s">
-        <v>518</v>
+        <v>529</v>
       </c>
       <c r="H78" t="s">
-        <v>408</v>
+        <v>555</v>
       </c>
       <c r="I78" t="s">
         <v>797</v>
@@ -4253,16 +4244,19 @@
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>134</v>
+        <v>89</v>
       </c>
       <c r="B79" t="s">
-        <v>528</v>
+        <v>535</v>
       </c>
       <c r="C79" s="7" t="s">
-        <v>519</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="D79" s="8"/>
+      <c r="E79" s="9"/>
+      <c r="F79" s="10"/>
       <c r="H79" t="s">
-        <v>520</v>
+        <v>536</v>
       </c>
       <c r="I79" t="s">
         <v>797</v>
@@ -4270,16 +4264,19 @@
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>530</v>
+        <v>543</v>
       </c>
       <c r="B80" t="s">
-        <v>531</v>
+        <v>538</v>
       </c>
       <c r="C80" s="7" t="s">
-        <v>529</v>
-      </c>
+        <v>537</v>
+      </c>
+      <c r="D80" s="8"/>
+      <c r="E80" s="9"/>
+      <c r="F80" s="10"/>
       <c r="H80" t="s">
-        <v>555</v>
+        <v>520</v>
       </c>
       <c r="I80" t="s">
         <v>797</v>
@@ -4290,7 +4287,7 @@
         <v>89</v>
       </c>
       <c r="B81" t="s">
-        <v>535</v>
+        <v>544</v>
       </c>
       <c r="C81" s="7" t="s">
         <v>111</v>
@@ -4299,7 +4296,7 @@
       <c r="E81" s="9"/>
       <c r="F81" s="10"/>
       <c r="H81" t="s">
-        <v>536</v>
+        <v>545</v>
       </c>
       <c r="I81" t="s">
         <v>797</v>
@@ -4307,13 +4304,13 @@
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>543</v>
+        <v>547</v>
       </c>
       <c r="B82" t="s">
-        <v>538</v>
+        <v>548</v>
       </c>
       <c r="C82" s="7" t="s">
-        <v>537</v>
+        <v>546</v>
       </c>
       <c r="D82" s="8"/>
       <c r="E82" s="9"/>
@@ -4330,7 +4327,7 @@
         <v>89</v>
       </c>
       <c r="B83" t="s">
-        <v>544</v>
+        <v>553</v>
       </c>
       <c r="C83" s="7" t="s">
         <v>111</v>
@@ -4339,7 +4336,7 @@
       <c r="E83" s="9"/>
       <c r="F83" s="10"/>
       <c r="H83" t="s">
-        <v>545</v>
+        <v>554</v>
       </c>
       <c r="I83" t="s">
         <v>797</v>
@@ -4347,53 +4344,47 @@
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>547</v>
+        <v>558</v>
       </c>
       <c r="B84" t="s">
-        <v>548</v>
+        <v>559</v>
       </c>
       <c r="C84" s="7" t="s">
-        <v>546</v>
+        <v>556</v>
       </c>
       <c r="D84" s="8"/>
       <c r="E84" s="9"/>
       <c r="F84" s="10"/>
-      <c r="H84" t="s">
-        <v>520</v>
-      </c>
       <c r="I84" t="s">
         <v>797</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>89</v>
+        <v>565</v>
       </c>
       <c r="B85" t="s">
-        <v>553</v>
+        <v>566</v>
       </c>
       <c r="C85" s="7" t="s">
-        <v>111</v>
+        <v>557</v>
       </c>
       <c r="D85" s="8"/>
       <c r="E85" s="9"/>
       <c r="F85" s="10"/>
-      <c r="H85" t="s">
-        <v>554</v>
-      </c>
       <c r="I85" t="s">
         <v>797</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>558</v>
+        <v>571</v>
       </c>
       <c r="B86" t="s">
-        <v>559</v>
+        <v>572</v>
       </c>
       <c r="C86" s="7" t="s">
-        <v>556</v>
+        <v>570</v>
       </c>
       <c r="D86" s="8"/>
       <c r="E86" s="9"/>
@@ -4404,13 +4395,13 @@
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>565</v>
+        <v>582</v>
       </c>
       <c r="B87" t="s">
-        <v>566</v>
+        <v>579</v>
       </c>
       <c r="C87" s="7" t="s">
-        <v>557</v>
+        <v>578</v>
       </c>
       <c r="D87" s="8"/>
       <c r="E87" s="9"/>
@@ -4419,15 +4410,15 @@
         <v>797</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>571</v>
+        <v>584</v>
       </c>
       <c r="B88" t="s">
-        <v>572</v>
+        <v>585</v>
       </c>
       <c r="C88" s="7" t="s">
-        <v>570</v>
+        <v>583</v>
       </c>
       <c r="D88" s="8"/>
       <c r="E88" s="9"/>
@@ -4436,16 +4427,11 @@
         <v>797</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
-        <v>582</v>
-      </c>
-      <c r="B89" t="s">
-        <v>579</v>
-      </c>
-      <c r="C89" s="7" t="s">
-        <v>578</v>
-      </c>
+    <row r="89" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="C89" s="7"/>
       <c r="D89" s="8"/>
       <c r="E89" s="9"/>
       <c r="F89" s="10"/>
@@ -4453,50 +4439,49 @@
         <v>797</v>
       </c>
     </row>
-    <row r="90" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
-        <v>584</v>
-      </c>
-      <c r="B90" t="s">
-        <v>585</v>
+    <row r="90" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B90" s="11" t="s">
+        <v>219</v>
       </c>
       <c r="C90" s="7" t="s">
-        <v>583</v>
+        <v>218</v>
       </c>
       <c r="D90" s="8"/>
       <c r="E90" s="9"/>
       <c r="F90" s="10"/>
+      <c r="H90" s="11" t="s">
+        <v>404</v>
+      </c>
       <c r="I90" t="s">
         <v>797</v>
       </c>
     </row>
-    <row r="91" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="16" t="s">
-        <v>107</v>
-      </c>
-      <c r="C91" s="7"/>
-      <c r="D91" s="8"/>
-      <c r="E91" s="9"/>
-      <c r="F91" s="10"/>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>153</v>
+      </c>
+      <c r="B91" t="s">
+        <v>593</v>
+      </c>
+      <c r="C91" s="7" t="s">
+        <v>590</v>
+      </c>
       <c r="I91" t="s">
         <v>797</v>
       </c>
     </row>
-    <row r="92" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B92" s="11" t="s">
-        <v>219</v>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>592</v>
+      </c>
+      <c r="B92" t="s">
+        <v>595</v>
       </c>
       <c r="C92" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="D92" s="8"/>
-      <c r="E92" s="9"/>
-      <c r="F92" s="10"/>
-      <c r="H92" s="11" t="s">
-        <v>404</v>
+        <v>591</v>
       </c>
       <c r="I92" t="s">
         <v>797</v>
@@ -4504,13 +4489,19 @@
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>153</v>
+        <v>89</v>
       </c>
       <c r="B93" t="s">
-        <v>593</v>
+        <v>610</v>
       </c>
       <c r="C93" s="7" t="s">
-        <v>590</v>
+        <v>111</v>
+      </c>
+      <c r="D93" s="8"/>
+      <c r="E93" s="9"/>
+      <c r="F93" s="10"/>
+      <c r="H93" t="s">
+        <v>611</v>
       </c>
       <c r="I93" t="s">
         <v>797</v>
@@ -4518,13 +4509,13 @@
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>592</v>
+        <v>613</v>
       </c>
       <c r="B94" t="s">
-        <v>595</v>
+        <v>614</v>
       </c>
       <c r="C94" s="7" t="s">
-        <v>591</v>
+        <v>612</v>
       </c>
       <c r="I94" t="s">
         <v>797</v>
@@ -4532,19 +4523,13 @@
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>89</v>
+        <v>134</v>
       </c>
       <c r="B95" t="s">
-        <v>610</v>
+        <v>618</v>
       </c>
       <c r="C95" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="D95" s="8"/>
-      <c r="E95" s="9"/>
-      <c r="F95" s="10"/>
-      <c r="H95" t="s">
-        <v>611</v>
+        <v>617</v>
       </c>
       <c r="I95" t="s">
         <v>797</v>
@@ -4552,13 +4537,16 @@
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>613</v>
+        <v>620</v>
       </c>
       <c r="B96" t="s">
-        <v>614</v>
+        <v>621</v>
       </c>
       <c r="C96" s="7" t="s">
-        <v>612</v>
+        <v>619</v>
+      </c>
+      <c r="H96" t="s">
+        <v>799</v>
       </c>
       <c r="I96" t="s">
         <v>797</v>
@@ -4566,13 +4554,19 @@
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>134</v>
+        <v>89</v>
       </c>
       <c r="B97" t="s">
-        <v>618</v>
+        <v>624</v>
       </c>
       <c r="C97" s="7" t="s">
-        <v>617</v>
+        <v>111</v>
+      </c>
+      <c r="D97" s="8"/>
+      <c r="E97" s="9"/>
+      <c r="F97" s="10"/>
+      <c r="H97" t="s">
+        <v>625</v>
       </c>
       <c r="I97" t="s">
         <v>797</v>
@@ -4580,16 +4574,13 @@
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>620</v>
+        <v>134</v>
       </c>
       <c r="B98" t="s">
-        <v>621</v>
+        <v>220</v>
       </c>
       <c r="C98" s="7" t="s">
-        <v>619</v>
-      </c>
-      <c r="H98" t="s">
-        <v>799</v>
+        <v>626</v>
       </c>
       <c r="I98" t="s">
         <v>797</v>
@@ -4597,19 +4588,16 @@
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>89</v>
+        <v>134</v>
       </c>
       <c r="B99" t="s">
-        <v>624</v>
+        <v>628</v>
       </c>
       <c r="C99" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="D99" s="8"/>
-      <c r="E99" s="9"/>
-      <c r="F99" s="10"/>
+        <v>627</v>
+      </c>
       <c r="H99" t="s">
-        <v>625</v>
+        <v>233</v>
       </c>
       <c r="I99" t="s">
         <v>797</v>
@@ -4617,13 +4605,16 @@
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>134</v>
+        <v>636</v>
       </c>
       <c r="B100" t="s">
-        <v>220</v>
+        <v>638</v>
       </c>
       <c r="C100" s="7" t="s">
-        <v>626</v>
+        <v>629</v>
+      </c>
+      <c r="H100" t="s">
+        <v>801</v>
       </c>
       <c r="I100" t="s">
         <v>797</v>
@@ -4631,16 +4622,19 @@
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>134</v>
+        <v>89</v>
       </c>
       <c r="B101" t="s">
-        <v>628</v>
+        <v>664</v>
       </c>
       <c r="C101" s="7" t="s">
-        <v>627</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="D101" s="8"/>
+      <c r="E101" s="9"/>
+      <c r="F101" s="10"/>
       <c r="H101" t="s">
-        <v>233</v>
+        <v>643</v>
       </c>
       <c r="I101" t="s">
         <v>797</v>
@@ -4648,16 +4642,16 @@
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>636</v>
+        <v>630</v>
       </c>
       <c r="B102" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="C102" s="7" t="s">
-        <v>629</v>
+        <v>635</v>
       </c>
       <c r="H102" t="s">
-        <v>801</v>
+        <v>663</v>
       </c>
       <c r="I102" t="s">
         <v>797</v>
@@ -4668,7 +4662,7 @@
         <v>89</v>
       </c>
       <c r="B103" t="s">
-        <v>664</v>
+        <v>634</v>
       </c>
       <c r="C103" s="7" t="s">
         <v>111</v>
@@ -4677,7 +4671,7 @@
       <c r="E103" s="9"/>
       <c r="F103" s="10"/>
       <c r="H103" t="s">
-        <v>643</v>
+        <v>800</v>
       </c>
       <c r="I103" t="s">
         <v>797</v>
@@ -4685,13 +4679,13 @@
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>630</v>
+        <v>646</v>
       </c>
       <c r="B104" t="s">
-        <v>637</v>
+        <v>645</v>
       </c>
       <c r="C104" s="7" t="s">
-        <v>635</v>
+        <v>644</v>
       </c>
       <c r="H104" t="s">
         <v>663</v>
@@ -4705,7 +4699,7 @@
         <v>89</v>
       </c>
       <c r="B105" t="s">
-        <v>634</v>
+        <v>652</v>
       </c>
       <c r="C105" s="7" t="s">
         <v>111</v>
@@ -4714,7 +4708,7 @@
       <c r="E105" s="9"/>
       <c r="F105" s="10"/>
       <c r="H105" t="s">
-        <v>800</v>
+        <v>653</v>
       </c>
       <c r="I105" t="s">
         <v>797</v>
@@ -4722,16 +4716,19 @@
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>646</v>
+        <v>134</v>
       </c>
       <c r="B106" t="s">
-        <v>645</v>
+        <v>655</v>
       </c>
       <c r="C106" s="7" t="s">
-        <v>644</v>
-      </c>
+        <v>654</v>
+      </c>
+      <c r="D106" s="8"/>
+      <c r="E106" s="9"/>
+      <c r="F106" s="10"/>
       <c r="H106" t="s">
-        <v>663</v>
+        <v>233</v>
       </c>
       <c r="I106" t="s">
         <v>797</v>
@@ -4739,88 +4736,73 @@
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>89</v>
+        <v>656</v>
       </c>
       <c r="B107" t="s">
-        <v>652</v>
+        <v>657</v>
       </c>
       <c r="C107" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="D107" s="8"/>
-      <c r="E107" s="9"/>
-      <c r="F107" s="10"/>
+        <v>658</v>
+      </c>
       <c r="H107" t="s">
-        <v>653</v>
+        <v>662</v>
       </c>
       <c r="I107" t="s">
         <v>797</v>
       </c>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
-        <v>134</v>
-      </c>
-      <c r="B108" t="s">
-        <v>655</v>
-      </c>
-      <c r="C108" s="7" t="s">
-        <v>654</v>
-      </c>
+    <row r="108" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="C108" s="7"/>
       <c r="D108" s="8"/>
       <c r="E108" s="9"/>
       <c r="F108" s="10"/>
-      <c r="H108" t="s">
-        <v>233</v>
-      </c>
       <c r="I108" t="s">
         <v>797</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A109" t="s">
-        <v>656</v>
-      </c>
-      <c r="B109" t="s">
-        <v>657</v>
+    <row r="109" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A109" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B109" s="11" t="s">
+        <v>234</v>
       </c>
       <c r="C109" s="7" t="s">
-        <v>658</v>
-      </c>
-      <c r="H109" t="s">
-        <v>662</v>
+        <v>235</v>
+      </c>
+      <c r="D109" s="8"/>
+      <c r="E109" s="9"/>
+      <c r="F109" s="10"/>
+      <c r="H109" s="11" t="s">
+        <v>665</v>
       </c>
       <c r="I109" t="s">
         <v>797</v>
       </c>
     </row>
-    <row r="110" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="16" t="s">
-        <v>107</v>
-      </c>
-      <c r="C110" s="7"/>
-      <c r="D110" s="8"/>
-      <c r="E110" s="9"/>
-      <c r="F110" s="10"/>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>103</v>
+      </c>
+      <c r="C110" t="s">
+        <v>236</v>
+      </c>
       <c r="I110" t="s">
         <v>797</v>
       </c>
     </row>
-    <row r="111" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B111" s="11" t="s">
-        <v>234</v>
-      </c>
-      <c r="C111" s="7" t="s">
-        <v>235</v>
-      </c>
-      <c r="D111" s="8"/>
-      <c r="E111" s="9"/>
-      <c r="F111" s="10"/>
-      <c r="H111" s="11" t="s">
-        <v>665</v>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>237</v>
+      </c>
+      <c r="B111" t="s">
+        <v>242</v>
+      </c>
+      <c r="C111" t="s">
+        <v>666</v>
       </c>
       <c r="I111" t="s">
         <v>797</v>
@@ -4828,10 +4810,13 @@
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>103</v>
+        <v>237</v>
+      </c>
+      <c r="B112" t="s">
+        <v>243</v>
       </c>
       <c r="C112" t="s">
-        <v>236</v>
+        <v>667</v>
       </c>
       <c r="I112" t="s">
         <v>797</v>
@@ -4842,10 +4827,10 @@
         <v>237</v>
       </c>
       <c r="B113" t="s">
-        <v>242</v>
+        <v>679</v>
       </c>
       <c r="C113" t="s">
-        <v>666</v>
+        <v>668</v>
       </c>
       <c r="I113" t="s">
         <v>797</v>
@@ -4856,10 +4841,10 @@
         <v>237</v>
       </c>
       <c r="B114" t="s">
-        <v>243</v>
+        <v>680</v>
       </c>
       <c r="C114" t="s">
-        <v>667</v>
+        <v>669</v>
       </c>
       <c r="I114" t="s">
         <v>797</v>
@@ -4870,10 +4855,10 @@
         <v>237</v>
       </c>
       <c r="B115" t="s">
-        <v>679</v>
+        <v>681</v>
       </c>
       <c r="C115" t="s">
-        <v>668</v>
+        <v>670</v>
       </c>
       <c r="I115" t="s">
         <v>797</v>
@@ -4884,10 +4869,10 @@
         <v>237</v>
       </c>
       <c r="B116" t="s">
-        <v>680</v>
+        <v>682</v>
       </c>
       <c r="C116" t="s">
-        <v>669</v>
+        <v>671</v>
       </c>
       <c r="I116" t="s">
         <v>797</v>
@@ -4898,10 +4883,10 @@
         <v>237</v>
       </c>
       <c r="B117" t="s">
-        <v>681</v>
+        <v>683</v>
       </c>
       <c r="C117" t="s">
-        <v>670</v>
+        <v>672</v>
       </c>
       <c r="I117" t="s">
         <v>797</v>
@@ -4912,10 +4897,10 @@
         <v>237</v>
       </c>
       <c r="B118" t="s">
-        <v>682</v>
+        <v>684</v>
       </c>
       <c r="C118" t="s">
-        <v>671</v>
+        <v>673</v>
       </c>
       <c r="I118" t="s">
         <v>797</v>
@@ -4926,10 +4911,10 @@
         <v>237</v>
       </c>
       <c r="B119" t="s">
-        <v>683</v>
+        <v>685</v>
       </c>
       <c r="C119" t="s">
-        <v>672</v>
+        <v>674</v>
       </c>
       <c r="I119" t="s">
         <v>797</v>
@@ -4940,10 +4925,10 @@
         <v>237</v>
       </c>
       <c r="B120" t="s">
-        <v>684</v>
+        <v>686</v>
       </c>
       <c r="C120" t="s">
-        <v>673</v>
+        <v>675</v>
       </c>
       <c r="I120" t="s">
         <v>797</v>
@@ -4954,10 +4939,10 @@
         <v>237</v>
       </c>
       <c r="B121" t="s">
-        <v>685</v>
+        <v>687</v>
       </c>
       <c r="C121" t="s">
-        <v>674</v>
+        <v>676</v>
       </c>
       <c r="I121" t="s">
         <v>797</v>
@@ -4965,13 +4950,13 @@
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>237</v>
+        <v>89</v>
       </c>
       <c r="B122" t="s">
-        <v>686</v>
+        <v>688</v>
       </c>
       <c r="C122" t="s">
-        <v>675</v>
+        <v>677</v>
       </c>
       <c r="I122" t="s">
         <v>797</v>
@@ -4982,10 +4967,10 @@
         <v>237</v>
       </c>
       <c r="B123" t="s">
-        <v>687</v>
+        <v>689</v>
       </c>
       <c r="C123" t="s">
-        <v>676</v>
+        <v>678</v>
       </c>
       <c r="I123" t="s">
         <v>797</v>
@@ -4993,13 +4978,16 @@
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>89</v>
+        <v>692</v>
       </c>
       <c r="B124" t="s">
-        <v>688</v>
+        <v>693</v>
       </c>
       <c r="C124" t="s">
-        <v>677</v>
+        <v>690</v>
+      </c>
+      <c r="H124" t="s">
+        <v>691</v>
       </c>
       <c r="I124" t="s">
         <v>797</v>
@@ -5007,13 +4995,19 @@
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>237</v>
+        <v>89</v>
       </c>
       <c r="B125" t="s">
-        <v>689</v>
-      </c>
-      <c r="C125" t="s">
-        <v>678</v>
+        <v>698</v>
+      </c>
+      <c r="C125" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="D125" s="8"/>
+      <c r="E125" s="9"/>
+      <c r="F125" s="10"/>
+      <c r="H125" t="s">
+        <v>699</v>
       </c>
       <c r="I125" t="s">
         <v>797</v>
@@ -5021,16 +5015,16 @@
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>692</v>
+        <v>244</v>
       </c>
       <c r="B126" t="s">
-        <v>693</v>
+        <v>258</v>
       </c>
       <c r="C126" t="s">
-        <v>690</v>
+        <v>700</v>
       </c>
       <c r="H126" t="s">
-        <v>691</v>
+        <v>701</v>
       </c>
       <c r="I126" t="s">
         <v>797</v>
@@ -5041,7 +5035,7 @@
         <v>89</v>
       </c>
       <c r="B127" t="s">
-        <v>698</v>
+        <v>275</v>
       </c>
       <c r="C127" s="7" t="s">
         <v>111</v>
@@ -5050,7 +5044,7 @@
       <c r="E127" s="9"/>
       <c r="F127" s="10"/>
       <c r="H127" t="s">
-        <v>699</v>
+        <v>276</v>
       </c>
       <c r="I127" t="s">
         <v>797</v>
@@ -5058,16 +5052,16 @@
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>244</v>
+        <v>256</v>
       </c>
       <c r="B128" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C128" t="s">
-        <v>700</v>
+        <v>703</v>
       </c>
       <c r="H128" t="s">
-        <v>701</v>
+        <v>702</v>
       </c>
       <c r="I128" t="s">
         <v>797</v>
@@ -5078,7 +5072,7 @@
         <v>89</v>
       </c>
       <c r="B129" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="C129" s="7" t="s">
         <v>111</v>
@@ -5087,7 +5081,7 @@
       <c r="E129" s="9"/>
       <c r="F129" s="10"/>
       <c r="H129" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="I129" t="s">
         <v>797</v>
@@ -5095,16 +5089,13 @@
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>256</v>
+        <v>261</v>
       </c>
       <c r="B130" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="C130" t="s">
-        <v>703</v>
-      </c>
-      <c r="H130" t="s">
-        <v>702</v>
+        <v>704</v>
       </c>
       <c r="I130" t="s">
         <v>797</v>
@@ -5115,7 +5106,7 @@
         <v>89</v>
       </c>
       <c r="B131" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="C131" s="7" t="s">
         <v>111</v>
@@ -5124,7 +5115,7 @@
       <c r="E131" s="9"/>
       <c r="F131" s="10"/>
       <c r="H131" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="I131" t="s">
         <v>797</v>
@@ -5132,13 +5123,13 @@
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>261</v>
+        <v>273</v>
       </c>
       <c r="B132" t="s">
-        <v>260</v>
+        <v>274</v>
       </c>
       <c r="C132" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
       <c r="I132" t="s">
         <v>797</v>
@@ -5146,19 +5137,16 @@
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>89</v>
+        <v>291</v>
       </c>
       <c r="B133" t="s">
-        <v>279</v>
-      </c>
-      <c r="C133" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="D133" s="8"/>
-      <c r="E133" s="9"/>
-      <c r="F133" s="10"/>
+        <v>290</v>
+      </c>
+      <c r="C133" t="s">
+        <v>706</v>
+      </c>
       <c r="H133" t="s">
-        <v>280</v>
+        <v>303</v>
       </c>
       <c r="I133" t="s">
         <v>797</v>
@@ -5166,13 +5154,19 @@
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>273</v>
+        <v>89</v>
       </c>
       <c r="B134" t="s">
-        <v>274</v>
-      </c>
-      <c r="C134" t="s">
-        <v>705</v>
+        <v>301</v>
+      </c>
+      <c r="C134" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="D134" s="8"/>
+      <c r="E134" s="9"/>
+      <c r="F134" s="10"/>
+      <c r="H134" t="s">
+        <v>302</v>
       </c>
       <c r="I134" t="s">
         <v>797</v>
@@ -5180,16 +5174,13 @@
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>291</v>
+        <v>305</v>
       </c>
       <c r="B135" t="s">
-        <v>290</v>
+        <v>304</v>
       </c>
       <c r="C135" t="s">
-        <v>706</v>
-      </c>
-      <c r="H135" t="s">
-        <v>303</v>
+        <v>707</v>
       </c>
       <c r="I135" t="s">
         <v>797</v>
@@ -5197,19 +5188,16 @@
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>89</v>
+        <v>153</v>
       </c>
       <c r="B136" t="s">
-        <v>301</v>
-      </c>
-      <c r="C136" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="D136" s="8"/>
-      <c r="E136" s="9"/>
-      <c r="F136" s="10"/>
-      <c r="H136" t="s">
-        <v>302</v>
+        <v>310</v>
+      </c>
+      <c r="C136" t="s">
+        <v>708</v>
+      </c>
+      <c r="D136" t="s">
+        <v>309</v>
       </c>
       <c r="I136" t="s">
         <v>797</v>
@@ -5217,13 +5205,16 @@
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>305</v>
+        <v>313</v>
       </c>
       <c r="B137" t="s">
-        <v>304</v>
+        <v>314</v>
       </c>
       <c r="C137" t="s">
-        <v>707</v>
+        <v>709</v>
+      </c>
+      <c r="H137" t="s">
+        <v>315</v>
       </c>
       <c r="I137" t="s">
         <v>797</v>
@@ -5231,16 +5222,16 @@
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>153</v>
+        <v>317</v>
       </c>
       <c r="B138" t="s">
-        <v>310</v>
+        <v>316</v>
       </c>
       <c r="C138" t="s">
-        <v>708</v>
-      </c>
-      <c r="D138" t="s">
-        <v>309</v>
+        <v>710</v>
+      </c>
+      <c r="H138" t="s">
+        <v>343</v>
       </c>
       <c r="I138" t="s">
         <v>797</v>
@@ -5248,16 +5239,19 @@
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>313</v>
+        <v>89</v>
       </c>
       <c r="B139" t="s">
-        <v>314</v>
-      </c>
-      <c r="C139" t="s">
-        <v>709</v>
-      </c>
+        <v>324</v>
+      </c>
+      <c r="C139" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="D139" s="8"/>
+      <c r="E139" s="9"/>
+      <c r="F139" s="10"/>
       <c r="H139" t="s">
-        <v>315</v>
+        <v>325</v>
       </c>
       <c r="I139" t="s">
         <v>797</v>
@@ -5265,16 +5259,16 @@
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>317</v>
+        <v>327</v>
       </c>
       <c r="B140" t="s">
-        <v>316</v>
+        <v>326</v>
       </c>
       <c r="C140" t="s">
-        <v>710</v>
+        <v>711</v>
       </c>
       <c r="H140" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="I140" t="s">
         <v>797</v>
@@ -5285,7 +5279,7 @@
         <v>89</v>
       </c>
       <c r="B141" t="s">
-        <v>324</v>
+        <v>340</v>
       </c>
       <c r="C141" s="7" t="s">
         <v>111</v>
@@ -5294,7 +5288,7 @@
       <c r="E141" s="9"/>
       <c r="F141" s="10"/>
       <c r="H141" t="s">
-        <v>325</v>
+        <v>341</v>
       </c>
       <c r="I141" t="s">
         <v>797</v>
@@ -5302,16 +5296,13 @@
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>327</v>
+        <v>237</v>
       </c>
       <c r="B142" t="s">
-        <v>326</v>
+        <v>344</v>
       </c>
       <c r="C142" t="s">
-        <v>711</v>
-      </c>
-      <c r="H142" t="s">
-        <v>342</v>
+        <v>712</v>
       </c>
       <c r="I142" t="s">
         <v>797</v>
@@ -5319,19 +5310,16 @@
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>89</v>
+        <v>345</v>
       </c>
       <c r="B143" t="s">
-        <v>340</v>
-      </c>
-      <c r="C143" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="D143" s="8"/>
-      <c r="E143" s="9"/>
-      <c r="F143" s="10"/>
+        <v>346</v>
+      </c>
+      <c r="C143" s="17" t="s">
+        <v>713</v>
+      </c>
       <c r="H143" t="s">
-        <v>341</v>
+        <v>353</v>
       </c>
       <c r="I143" t="s">
         <v>797</v>
@@ -5339,13 +5327,19 @@
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>237</v>
+        <v>89</v>
       </c>
       <c r="B144" t="s">
-        <v>344</v>
-      </c>
-      <c r="C144" t="s">
-        <v>712</v>
+        <v>354</v>
+      </c>
+      <c r="C144" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="D144" s="8"/>
+      <c r="E144" s="9"/>
+      <c r="F144" s="10"/>
+      <c r="H144" t="s">
+        <v>355</v>
       </c>
       <c r="I144" t="s">
         <v>797</v>
@@ -5353,84 +5347,75 @@
     </row>
     <row r="145" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>345</v>
+        <v>720</v>
       </c>
       <c r="B145" t="s">
-        <v>346</v>
-      </c>
-      <c r="C145" s="17" t="s">
-        <v>713</v>
-      </c>
-      <c r="H145" t="s">
-        <v>353</v>
-      </c>
+        <v>715</v>
+      </c>
+      <c r="C145" s="7" t="s">
+        <v>714</v>
+      </c>
+      <c r="D145" s="8"/>
+      <c r="E145" s="9"/>
+      <c r="F145" s="10"/>
       <c r="I145" t="s">
         <v>797</v>
       </c>
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>89</v>
+        <v>153</v>
       </c>
       <c r="B146" t="s">
-        <v>354</v>
+        <v>722</v>
       </c>
       <c r="C146" s="7" t="s">
-        <v>111</v>
+        <v>721</v>
       </c>
       <c r="D146" s="8"/>
       <c r="E146" s="9"/>
       <c r="F146" s="10"/>
-      <c r="H146" t="s">
-        <v>355</v>
-      </c>
       <c r="I146" t="s">
         <v>797</v>
       </c>
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>720</v>
+        <v>237</v>
       </c>
       <c r="B147" t="s">
-        <v>715</v>
-      </c>
-      <c r="C147" s="7" t="s">
-        <v>714</v>
-      </c>
-      <c r="D147" s="8"/>
-      <c r="E147" s="9"/>
-      <c r="F147" s="10"/>
+        <v>356</v>
+      </c>
+      <c r="C147" t="s">
+        <v>723</v>
+      </c>
       <c r="I147" t="s">
         <v>797</v>
       </c>
     </row>
     <row r="148" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>153</v>
+        <v>237</v>
       </c>
       <c r="B148" t="s">
-        <v>722</v>
-      </c>
-      <c r="C148" s="7" t="s">
-        <v>721</v>
-      </c>
-      <c r="D148" s="8"/>
-      <c r="E148" s="9"/>
-      <c r="F148" s="10"/>
+        <v>360</v>
+      </c>
+      <c r="C148" t="s">
+        <v>724</v>
+      </c>
       <c r="I148" t="s">
         <v>797</v>
       </c>
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>237</v>
+        <v>153</v>
       </c>
       <c r="B149" t="s">
-        <v>356</v>
-      </c>
-      <c r="C149" t="s">
-        <v>723</v>
+        <v>726</v>
+      </c>
+      <c r="C149" s="7" t="s">
+        <v>725</v>
       </c>
       <c r="I149" t="s">
         <v>797</v>
@@ -5438,13 +5423,13 @@
     </row>
     <row r="150" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>237</v>
+        <v>730</v>
       </c>
       <c r="B150" t="s">
-        <v>360</v>
-      </c>
-      <c r="C150" t="s">
-        <v>724</v>
+        <v>728</v>
+      </c>
+      <c r="C150" s="7" t="s">
+        <v>727</v>
       </c>
       <c r="I150" t="s">
         <v>797</v>
@@ -5452,13 +5437,16 @@
     </row>
     <row r="151" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>153</v>
+        <v>361</v>
       </c>
       <c r="B151" t="s">
-        <v>726</v>
-      </c>
-      <c r="C151" s="7" t="s">
-        <v>725</v>
+        <v>362</v>
+      </c>
+      <c r="C151" t="s">
+        <v>731</v>
+      </c>
+      <c r="H151" t="s">
+        <v>366</v>
       </c>
       <c r="I151" t="s">
         <v>797</v>
@@ -5466,13 +5454,13 @@
     </row>
     <row r="152" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>730</v>
+        <v>734</v>
       </c>
       <c r="B152" t="s">
-        <v>728</v>
+        <v>736</v>
       </c>
       <c r="C152" s="7" t="s">
-        <v>727</v>
+        <v>733</v>
       </c>
       <c r="I152" t="s">
         <v>797</v>
@@ -5480,16 +5468,19 @@
     </row>
     <row r="153" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>361</v>
+        <v>89</v>
       </c>
       <c r="B153" t="s">
-        <v>362</v>
-      </c>
-      <c r="C153" t="s">
-        <v>731</v>
-      </c>
+        <v>750</v>
+      </c>
+      <c r="C153" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="D153" s="8"/>
+      <c r="E153" s="9"/>
+      <c r="F153" s="10"/>
       <c r="H153" t="s">
-        <v>366</v>
+        <v>751</v>
       </c>
       <c r="I153" t="s">
         <v>797</v>
@@ -5497,33 +5488,36 @@
     </row>
     <row r="154" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>734</v>
+        <v>153</v>
       </c>
       <c r="B154" t="s">
-        <v>736</v>
+        <v>753</v>
       </c>
       <c r="C154" s="7" t="s">
-        <v>733</v>
-      </c>
+        <v>752</v>
+      </c>
+      <c r="D154" s="8"/>
+      <c r="E154" s="9"/>
+      <c r="F154" s="10"/>
       <c r="I154" t="s">
         <v>797</v>
       </c>
     </row>
     <row r="155" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>89</v>
+        <v>153</v>
       </c>
       <c r="B155" t="s">
-        <v>750</v>
+        <v>755</v>
       </c>
       <c r="C155" s="7" t="s">
-        <v>111</v>
+        <v>754</v>
       </c>
       <c r="D155" s="8"/>
       <c r="E155" s="9"/>
       <c r="F155" s="10"/>
       <c r="H155" t="s">
-        <v>751</v>
+        <v>756</v>
       </c>
       <c r="I155" t="s">
         <v>797</v>
@@ -5531,36 +5525,39 @@
     </row>
     <row r="156" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>153</v>
+        <v>758</v>
       </c>
       <c r="B156" t="s">
-        <v>753</v>
+        <v>759</v>
       </c>
       <c r="C156" s="7" t="s">
-        <v>752</v>
+        <v>757</v>
       </c>
       <c r="D156" s="8"/>
       <c r="E156" s="9"/>
       <c r="F156" s="10"/>
+      <c r="H156" t="s">
+        <v>769</v>
+      </c>
       <c r="I156" t="s">
         <v>797</v>
       </c>
     </row>
     <row r="157" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>153</v>
+        <v>89</v>
       </c>
       <c r="B157" t="s">
-        <v>755</v>
+        <v>767</v>
       </c>
       <c r="C157" s="7" t="s">
-        <v>754</v>
+        <v>111</v>
       </c>
       <c r="D157" s="8"/>
       <c r="E157" s="9"/>
       <c r="F157" s="10"/>
       <c r="H157" t="s">
-        <v>756</v>
+        <v>768</v>
       </c>
       <c r="I157" t="s">
         <v>797</v>
@@ -5568,19 +5565,13 @@
     </row>
     <row r="158" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>758</v>
+        <v>367</v>
       </c>
       <c r="B158" t="s">
-        <v>759</v>
-      </c>
-      <c r="C158" s="7" t="s">
-        <v>757</v>
-      </c>
-      <c r="D158" s="8"/>
-      <c r="E158" s="9"/>
-      <c r="F158" s="10"/>
-      <c r="H158" t="s">
-        <v>769</v>
+        <v>368</v>
+      </c>
+      <c r="C158" t="s">
+        <v>770</v>
       </c>
       <c r="I158" t="s">
         <v>797</v>
@@ -5588,19 +5579,13 @@
     </row>
     <row r="159" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>89</v>
+        <v>153</v>
       </c>
       <c r="B159" t="s">
-        <v>767</v>
-      </c>
-      <c r="C159" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="D159" s="8"/>
-      <c r="E159" s="9"/>
-      <c r="F159" s="10"/>
-      <c r="H159" t="s">
-        <v>768</v>
+        <v>772</v>
+      </c>
+      <c r="C159" t="s">
+        <v>771</v>
       </c>
       <c r="I159" t="s">
         <v>797</v>
@@ -5608,13 +5593,16 @@
     </row>
     <row r="160" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>367</v>
+        <v>153</v>
       </c>
       <c r="B160" t="s">
-        <v>368</v>
+        <v>774</v>
       </c>
       <c r="C160" t="s">
-        <v>770</v>
+        <v>773</v>
+      </c>
+      <c r="H160" t="s">
+        <v>775</v>
       </c>
       <c r="I160" t="s">
         <v>797</v>
@@ -5622,13 +5610,13 @@
     </row>
     <row r="161" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>153</v>
+        <v>392</v>
       </c>
       <c r="B161" t="s">
-        <v>772</v>
+        <v>379</v>
       </c>
       <c r="C161" t="s">
-        <v>771</v>
+        <v>776</v>
       </c>
       <c r="I161" t="s">
         <v>797</v>
@@ -5636,16 +5624,19 @@
     </row>
     <row r="162" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>153</v>
+        <v>89</v>
       </c>
       <c r="B162" t="s">
-        <v>774</v>
-      </c>
-      <c r="C162" t="s">
-        <v>773</v>
-      </c>
+        <v>383</v>
+      </c>
+      <c r="C162" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="D162" s="8"/>
+      <c r="E162" s="9"/>
+      <c r="F162" s="10"/>
       <c r="H162" t="s">
-        <v>775</v>
+        <v>384</v>
       </c>
       <c r="I162" t="s">
         <v>797</v>
@@ -5653,13 +5644,13 @@
     </row>
     <row r="163" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>392</v>
+        <v>135</v>
       </c>
       <c r="B163" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="C163" t="s">
-        <v>776</v>
+        <v>777</v>
       </c>
       <c r="I163" t="s">
         <v>797</v>
@@ -5667,19 +5658,13 @@
     </row>
     <row r="164" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>89</v>
+        <v>135</v>
       </c>
       <c r="B164" t="s">
-        <v>383</v>
-      </c>
-      <c r="C164" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="D164" s="8"/>
-      <c r="E164" s="9"/>
-      <c r="F164" s="10"/>
-      <c r="H164" t="s">
-        <v>384</v>
+        <v>381</v>
+      </c>
+      <c r="C164" t="s">
+        <v>778</v>
       </c>
       <c r="I164" t="s">
         <v>797</v>
@@ -5690,79 +5675,81 @@
         <v>135</v>
       </c>
       <c r="B165" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="C165" t="s">
-        <v>777</v>
+        <v>779</v>
       </c>
       <c r="I165" t="s">
         <v>797</v>
       </c>
     </row>
-    <row r="166" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A166" t="s">
-        <v>135</v>
-      </c>
-      <c r="B166" t="s">
-        <v>381</v>
-      </c>
-      <c r="C166" t="s">
-        <v>778</v>
-      </c>
+    <row r="166" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A166" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="C166" s="7"/>
+      <c r="D166" s="8"/>
+      <c r="E166" s="9"/>
+      <c r="F166" s="10"/>
       <c r="I166" t="s">
         <v>797</v>
       </c>
     </row>
-    <row r="167" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A167" t="s">
-        <v>135</v>
-      </c>
-      <c r="B167" t="s">
-        <v>382</v>
-      </c>
-      <c r="C167" t="s">
-        <v>779</v>
+    <row r="167" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A167" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B167" s="11" t="s">
+        <v>780</v>
+      </c>
+      <c r="C167" s="21" t="s">
+        <v>781</v>
+      </c>
+      <c r="D167" s="21"/>
+      <c r="H167" s="11" t="s">
+        <v>110</v>
       </c>
       <c r="I167" t="s">
         <v>797</v>
       </c>
     </row>
-    <row r="168" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A168" s="16" t="s">
-        <v>107</v>
-      </c>
-      <c r="C168" s="7"/>
-      <c r="D168" s="8"/>
-      <c r="E168" s="9"/>
-      <c r="F168" s="10"/>
+    <row r="168" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A168" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="C168" s="20" t="s">
+        <v>782</v>
+      </c>
+      <c r="D168" s="20"/>
       <c r="I168" t="s">
         <v>797</v>
       </c>
     </row>
-    <row r="169" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A169" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B169" s="11" t="s">
-        <v>780</v>
-      </c>
-      <c r="C169" s="21" t="s">
-        <v>781</v>
-      </c>
-      <c r="D169" s="21"/>
-      <c r="H169" s="11" t="s">
-        <v>110</v>
-      </c>
+    <row r="169" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A169" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="B169" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="C169" s="20" t="s">
+        <v>784</v>
+      </c>
+      <c r="D169" s="20"/>
       <c r="I169" t="s">
         <v>797</v>
       </c>
     </row>
     <row r="170" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A170" s="19" t="s">
-        <v>103</v>
+        <v>121</v>
+      </c>
+      <c r="B170" s="19" t="s">
+        <v>783</v>
       </c>
       <c r="C170" s="20" t="s">
-        <v>782</v>
+        <v>785</v>
       </c>
       <c r="D170" s="20"/>
       <c r="I170" t="s">
@@ -5771,88 +5758,95 @@
     </row>
     <row r="171" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A171" s="19" t="s">
-        <v>121</v>
+        <v>134</v>
       </c>
       <c r="B171" s="19" t="s">
-        <v>122</v>
+        <v>402</v>
       </c>
       <c r="C171" s="20" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D171" s="20"/>
       <c r="I171" t="s">
         <v>797</v>
       </c>
     </row>
-    <row r="172" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A172" s="19" t="s">
-        <v>121</v>
-      </c>
-      <c r="B172" s="19" t="s">
-        <v>783</v>
-      </c>
-      <c r="C172" s="20" t="s">
-        <v>785</v>
-      </c>
-      <c r="D172" s="20"/>
+    <row r="172" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
+        <v>89</v>
+      </c>
+      <c r="B172" t="s">
+        <v>787</v>
+      </c>
+      <c r="C172" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="D172" s="8"/>
+      <c r="E172" s="9"/>
+      <c r="F172" s="10"/>
+      <c r="H172" t="s">
+        <v>788</v>
+      </c>
       <c r="I172" t="s">
         <v>797</v>
       </c>
     </row>
-    <row r="173" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A173" s="19" t="s">
-        <v>134</v>
-      </c>
-      <c r="B173" s="19" t="s">
-        <v>402</v>
-      </c>
-      <c r="C173" s="20" t="s">
-        <v>786</v>
-      </c>
-      <c r="D173" s="20"/>
+    <row r="173" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A173" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="C173" s="22"/>
+      <c r="D173" s="22"/>
       <c r="I173" t="s">
         <v>797</v>
       </c>
     </row>
     <row r="174" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>89</v>
+        <v>385</v>
       </c>
       <c r="B174" t="s">
-        <v>787</v>
+        <v>79</v>
       </c>
       <c r="C174" s="7" t="s">
-        <v>111</v>
+        <v>386</v>
       </c>
       <c r="D174" s="8"/>
       <c r="E174" s="9"/>
       <c r="F174" s="10"/>
-      <c r="H174" t="s">
-        <v>788</v>
-      </c>
       <c r="I174" t="s">
         <v>797</v>
       </c>
     </row>
-    <row r="175" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A175" s="16" t="s">
-        <v>107</v>
-      </c>
-      <c r="C175" s="22"/>
-      <c r="D175" s="22"/>
+    <row r="175" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
+        <v>89</v>
+      </c>
+      <c r="B175" t="s">
+        <v>403</v>
+      </c>
+      <c r="C175" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="D175" s="8"/>
+      <c r="E175" s="9"/>
+      <c r="F175" s="10"/>
+      <c r="H175" t="s">
+        <v>387</v>
+      </c>
       <c r="I175" t="s">
         <v>797</v>
       </c>
     </row>
     <row r="176" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>385</v>
+        <v>89</v>
       </c>
       <c r="B176" t="s">
-        <v>79</v>
+        <v>388</v>
       </c>
       <c r="C176" s="7" t="s">
-        <v>386</v>
+        <v>389</v>
       </c>
       <c r="D176" s="8"/>
       <c r="E176" s="9"/>
@@ -5863,55 +5857,18 @@
     </row>
     <row r="177" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>89</v>
+        <v>100</v>
       </c>
       <c r="B177" t="s">
-        <v>403</v>
+        <v>390</v>
       </c>
       <c r="C177" s="7" t="s">
-        <v>85</v>
+        <v>391</v>
       </c>
       <c r="D177" s="8"/>
       <c r="E177" s="9"/>
       <c r="F177" s="10"/>
-      <c r="H177" t="s">
-        <v>387</v>
-      </c>
       <c r="I177" t="s">
-        <v>797</v>
-      </c>
-    </row>
-    <row r="178" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A178" t="s">
-        <v>89</v>
-      </c>
-      <c r="B178" t="s">
-        <v>388</v>
-      </c>
-      <c r="C178" s="7" t="s">
-        <v>389</v>
-      </c>
-      <c r="D178" s="8"/>
-      <c r="E178" s="9"/>
-      <c r="F178" s="10"/>
-      <c r="I178" t="s">
-        <v>797</v>
-      </c>
-    </row>
-    <row r="179" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A179" t="s">
-        <v>100</v>
-      </c>
-      <c r="B179" t="s">
-        <v>390</v>
-      </c>
-      <c r="C179" s="7" t="s">
-        <v>391</v>
-      </c>
-      <c r="D179" s="8"/>
-      <c r="E179" s="9"/>
-      <c r="F179" s="10"/>
-      <c r="I179" t="s">
         <v>797</v>
       </c>
     </row>

</xml_diff>